<commit_message>
Button add and edit Registries added
</commit_message>
<xml_diff>
--- a/Registro.xlsx
+++ b/Registro.xlsx
@@ -47,98 +47,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -330,14 +240,14 @@
     <row r="2" customHeight="true" ht="20.0">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>2018-11-17</t>
+          <t>2018-12-04</t>
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="C2" s="9" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>0.0</v>
@@ -346,20 +256,20 @@
         <v>0.0</v>
       </c>
       <c r="F2" s="12" t="n">
-        <v>33.333333333333336</v>
+        <v>28.125000000000004</v>
       </c>
     </row>
     <row r="3" customHeight="true" ht="20.0">
       <c r="A3" s="13" t="inlineStr">
         <is>
-          <t>2018-11-17</t>
+          <t>2018-12-10</t>
         </is>
       </c>
       <c r="B3" s="14" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="D3" s="16" t="n">
         <v>0.0</v>
@@ -368,20 +278,20 @@
         <v>0.0</v>
       </c>
       <c r="F3" s="18" t="n">
-        <v>33.333333333333336</v>
+        <v>22.500000000000004</v>
       </c>
     </row>
     <row r="4" customHeight="true" ht="20.0">
       <c r="A4" s="19" t="inlineStr">
         <is>
-          <t>2018-11-29</t>
+          <t>2018-12-11</t>
         </is>
       </c>
       <c r="B4" s="20" t="n">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="C4" s="21" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="D4" s="22" t="n">
         <v>0.0</v>
@@ -390,20 +300,20 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="24" t="n">
-        <v>91.66666666666667</v>
+        <v>22.500000000000004</v>
       </c>
     </row>
     <row r="5" customHeight="true" ht="20.0">
       <c r="A5" s="25" t="inlineStr">
         <is>
-          <t>2018-11-29</t>
+          <t>2018-12-12</t>
         </is>
       </c>
       <c r="B5" s="26" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" s="27" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="D5" s="28" t="n">
         <v>0.0</v>
@@ -412,42 +322,42 @@
         <v>0.0</v>
       </c>
       <c r="F5" s="30" t="n">
-        <v>91.66666666666667</v>
+        <v>39.16666666666667</v>
       </c>
     </row>
     <row r="6" customHeight="true" ht="20.0">
       <c r="A6" s="31" t="inlineStr">
         <is>
-          <t>2018-11-17</t>
+          <t>2018-12-13</t>
         </is>
       </c>
       <c r="B6" s="32" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" s="33" t="n">
         <v>5.0</v>
       </c>
       <c r="D6" s="34" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="E6" s="35" t="n">
         <v>0.0</v>
       </c>
       <c r="F6" s="36" t="n">
-        <v>169.79166666666669</v>
+        <v>32.29166666666667</v>
       </c>
     </row>
     <row r="7" customHeight="true" ht="20.0">
       <c r="A7" s="37" t="inlineStr">
         <is>
-          <t>2018-11-22</t>
+          <t>2018-12-14</t>
         </is>
       </c>
       <c r="B7" s="38" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C7" s="39" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="D7" s="40" t="n">
         <v>0.0</v>
@@ -456,139 +366,29 @@
         <v>0.0</v>
       </c>
       <c r="F7" s="42" t="n">
-        <v>197.91666666666669</v>
+        <v>30.833333333333336</v>
       </c>
     </row>
     <row r="8" customHeight="true" ht="20.0">
       <c r="A8" s="43" t="inlineStr">
         <is>
-          <t>2018-11-21</t>
+          <t>TOTAL:</t>
         </is>
       </c>
       <c r="B8" s="44" t="n">
         <v>7.0</v>
       </c>
       <c r="C8" s="45" t="n">
-        <v>1.0</v>
+        <v>26.0</v>
       </c>
       <c r="D8" s="46" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="E8" s="47" t="n">
         <v>0.0</v>
       </c>
       <c r="F8" s="48" t="n">
-        <v>55.62500000000001</v>
-      </c>
-    </row>
-    <row r="9" customHeight="true" ht="20.0">
-      <c r="A9" s="49" t="inlineStr">
-        <is>
-          <t>2018-11-7</t>
-        </is>
-      </c>
-      <c r="B9" s="50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C9" s="51" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D9" s="52" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="53" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="F9" s="54" t="n">
-        <v>187.5</v>
-      </c>
-    </row>
-    <row r="10" customHeight="true" ht="20.0">
-      <c r="A10" s="55" t="inlineStr">
-        <is>
-          <t>2018-11-30</t>
-        </is>
-      </c>
-      <c r="B10" s="56" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C10" s="57" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D10" s="58" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="E10" s="59" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="F10" s="60" t="n">
-        <v>304.1666666666667</v>
-      </c>
-    </row>
-    <row r="11" customHeight="true" ht="20.0">
-      <c r="A11" s="61" t="inlineStr">
-        <is>
-          <t>2018-11-18</t>
-        </is>
-      </c>
-      <c r="B11" s="62" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C11" s="63" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D11" s="64" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E11" s="65" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F11" s="66" t="n">
-        <v>22.291666666666668</v>
-      </c>
-    </row>
-    <row r="12" customHeight="true" ht="20.0">
-      <c r="A12" s="67" t="inlineStr">
-        <is>
-          <t>2018-11-20</t>
-        </is>
-      </c>
-      <c r="B12" s="68" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="C12" s="69" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="D12" s="70" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E12" s="71" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="F12" s="72" t="n">
-        <v>68.75</v>
-      </c>
-    </row>
-    <row r="13" customHeight="true" ht="20.0">
-      <c r="A13" s="73" t="inlineStr">
-        <is>
-          <t>TOTAL:</t>
-        </is>
-      </c>
-      <c r="B13" s="74" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="C13" s="75" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="D13" s="76" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="E13" s="77" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="F13" s="78" t="n">
-        <v>1256.0416666666667</v>
+        <v>175.4166666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>